<commit_message>
fix: use id 1-7 for ranks to support cms
</commit_message>
<xml_diff>
--- a/arcturus/perms.xlsx
+++ b/arcturus/perms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikla\Documents\Projekte\nitro\arcturus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A62EDF-CC29-4B35-B485-6E4B68E50E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD556BC-C237-4B90-856E-0F69343A8C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C8B827B5-A31F-45DA-B9D1-B0119BBAA915}"/>
   </bookViews>
@@ -942,7 +942,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,25 +1015,25 @@
         <v>163</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E3">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="F3">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G3">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H3">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>